<commit_message>
added more feature and UI
</commit_message>
<xml_diff>
--- a/Pace Supply/Pace Supply/edi_mapping_generator/input/inbound_X12_to_oracle.xlsx
+++ b/Pace Supply/Pace Supply/edi_mapping_generator/input/inbound_X12_to_oracle.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="460">
   <si>
     <t xml:space="preserve">ELECTRONIC DATA INTERCHANGE (EDI) LAYOUT DOCUMENT</t>
   </si>
@@ -352,27 +352,50 @@
     <t xml:space="preserve">VARCHAR2</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'ED'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test_Indicator</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'T' or 'P'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Document_ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'POI'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Document_Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'STAND'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Document_Purpose_Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'OR'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Document_Code</t>
   </si>
   <si>
     <t xml:space="preserve">TP_Translator_Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Sender ID GS02</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP_Location_Code</t>
   </si>
   <si>
+    <t xml:space="preserve">If BEG02!= DS, then capture N104 of N1*ST loop
+If BEG02=DS, then capture "N1*02 of N1*ST loop( first 3 characters)"+"_"+"N3*01(first 5 characters)+"_"+"N4*03(first5characters)" making a total max legth of 15 characters. 
+Note -- Remove any spaces if you find in N1*02 or N3*01or N4*03</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP_Description</t>
   </si>
   <si>
@@ -388,6 +411,9 @@
     <t xml:space="preserve">DATE</t>
   </si>
   <si>
+    <t xml:space="preserve">Update with System Date - YYYYMMDD HHMMSS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Transaction_Run_ID</t>
   </si>
   <si>
@@ -403,12 +429,21 @@
     <t xml:space="preserve">CONTROL1</t>
   </si>
   <si>
+    <t xml:space="preserve">ISA Control Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONTROL2</t>
   </si>
   <si>
+    <t xml:space="preserve">GS Control Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONTROL3</t>
   </si>
   <si>
+    <t xml:space="preserve">ST  Control Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">0020 Record</t>
   </si>
   <si>
@@ -421,9 +456,18 @@
     <t xml:space="preserve">TP_ATTRIBUTE_1</t>
   </si>
   <si>
+    <t xml:space="preserve">Sender ID GS02 (TO BE REVIEWED) Use one value for each customer
+Use one constant value for the each trading partner</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP_ATTRIBUTE_2</t>
   </si>
   <si>
+    <t xml:space="preserve">Please add the logic When BEG02=DS then capture "N1*02 of N1*ST loop( first 3 characters)"+"_"+"N3*01(first 5 characters)+"_"+"N4*03(first5characters)" making a total max legth of 15 characters. 
+Note -- Remove any spaces if you find in N1*02 or N3*01or N4*03
+When BEG02!=DS, then capture N104 of N1*ST loop</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP_ATTRIBUTE_3</t>
   </si>
   <si>
@@ -442,21 +486,33 @@
     <t xml:space="preserve">OPERATION_CODE</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'INSERT'</t>
+  </si>
+  <si>
     <t xml:space="preserve">OPERATION_CODE_EXT1</t>
   </si>
   <si>
     <t xml:space="preserve">CUSTOMER_PO_NUMBER</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer PO Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">ORDERED_DATE</t>
   </si>
   <si>
+    <t xml:space="preserve">If present in BEG05, else Update with System Date - YYYYMMDD HHMMSS</t>
+  </si>
+  <si>
     <t xml:space="preserve">VERSION_NUMBER</t>
   </si>
   <si>
     <t xml:space="preserve">Order_Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'Order'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Order_Type_Ext1</t>
   </si>
   <si>
@@ -487,6 +543,9 @@
     <t xml:space="preserve">BOOKED_FLAG</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant value of 'Y'</t>
+  </si>
+  <si>
     <t xml:space="preserve">1060 Record</t>
   </si>
   <si>
@@ -598,9 +657,15 @@
     <t xml:space="preserve">Shipping_Instructions_A</t>
   </si>
   <si>
+    <t xml:space="preserve">If the value in MSG01 exists, Map all the MSG01 values received in the Purchase Order sepearated by spaces</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shipping_Instructions_B</t>
   </si>
   <si>
+    <t xml:space="preserve">WHEN REF*Q1 exists:map the value as "Quote Number: " + REF02</t>
+  </si>
+  <si>
     <t xml:space="preserve">1110 Record</t>
   </si>
   <si>
@@ -608,6 +673,9 @@
   </si>
   <si>
     <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualifier 002</t>
   </si>
   <si>
     <t xml:space="preserve">1200 Record</t>
@@ -639,6 +707,11 @@
  </t>
   </si>
   <si>
+    <t xml:space="preserve">Please add the logic When BEG02=DS then capture "N1*02( first 3 characters)"+"_"+"N3*01(first 5 characters)+"_"+"N4*03(first5characters)" making a total max legth of 15 characters. 
+Note -- Remove any spaces if you find in N1*02 or N3*01or N4*03
+When BEG02!=DS, then capture N104 of N1*ST loop</t>
+  </si>
+  <si>
     <t xml:space="preserve">PO Header Attribute 6
 </t>
   </si>
@@ -664,6 +737,9 @@
     <t xml:space="preserve">SOLD_TO_EDI_Location_Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Use TP Table based on Sender ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOLD_TO_ADDRESS_NAME</t>
   </si>
   <si>
@@ -769,21 +845,35 @@
     <t xml:space="preserve">2000 Record</t>
   </si>
   <si>
+    <t xml:space="preserve">PO Line Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Customer_Line_Number</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer PO Line Number (start col 101)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Line_Number</t>
   </si>
   <si>
     <t xml:space="preserve">Inventory_Item</t>
   </si>
   <si>
+    <t xml:space="preserve">If customer supplied VC, VN, or VP then populate else Leave NULL: 
+It has the VC, VN, or VP vendor part if cust</t>
+  </si>
+  <si>
     <t xml:space="preserve">Item_Revision</t>
   </si>
   <si>
     <t xml:space="preserve">Customer_Item_Name</t>
   </si>
   <si>
+    <t xml:space="preserve">If PO108 = BP then populate with PO109
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Customer_Item_Revision</t>
   </si>
   <si>
@@ -796,9 +886,16 @@
     <t xml:space="preserve">Orig_Sys_Document_Ref</t>
   </si>
   <si>
+    <t xml:space="preserve">See ORIG_SYS_REF tab 
+(CUST3 || '-' || Customer PO) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Orig_Sys_Line_Ref</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer PO Line Number </t>
+  </si>
+  <si>
     <t xml:space="preserve">Item_Type_Code</t>
   </si>
   <si>
@@ -814,6 +911,9 @@
     <t xml:space="preserve">Calculate_Price_Flag</t>
   </si>
   <si>
+    <t xml:space="preserve">Constant 'Y'.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pricing_Quantity</t>
   </si>
   <si>
@@ -892,12 +992,19 @@
     <t xml:space="preserve">Customer_Shipment_Number</t>
   </si>
   <si>
+    <t xml:space="preserve">Sequential Number if there are multiple shipments per PO1 segment.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orig_Sys_Shipment_Ref</t>
   </si>
   <si>
     <t xml:space="preserve">Request_Date</t>
   </si>
   <si>
+    <t xml:space="preserve">Ship Date from Header if one is not found on the line.
+Otherwise, this is the line level requested ship date.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Schedule_Date</t>
   </si>
   <si>
@@ -910,9 +1017,15 @@
     <t xml:space="preserve">Ordered_Quantity</t>
   </si>
   <si>
+    <t xml:space="preserve">Line Item Quantity</t>
+  </si>
+  <si>
     <t xml:space="preserve">Order_Quantity_UOM</t>
   </si>
   <si>
+    <t xml:space="preserve">UOM is 'EA' - Validate UOM Codes in Table</t>
+  </si>
+  <si>
     <t xml:space="preserve">Order_Quantity_UOM_EXT1</t>
   </si>
   <si>
@@ -956,6 +1069,9 @@
   </si>
   <si>
     <t xml:space="preserve">4800 Record </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDI Location code N104 with ST Qualifier</t>
   </si>
   <si>
     <t xml:space="preserve">S168583X                 8860                                                              0010CTCTLEDPPOI   STANDOR                                   TC1000                        TL1000                                                                                                                                                                                                                                                                       20100525 142522000000000000000                         09876543211234567890ABCDEFGHIJ</t>
@@ -1606,7 +1722,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="116">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1951,10 +2067,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2020,23 +2132,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2174,9 +2270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2367720</xdr:colOff>
+      <xdr:colOff>2367000</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2190,7 +2286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7229520"/>
-          <a:ext cx="4272840" cy="1051200"/>
+          <a:ext cx="4272120" cy="1050480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2216,7 +2312,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.56"/>
@@ -2322,9 +2418,9 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="19.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.66"/>
@@ -2333,7 +2429,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.35"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3735,23 +3831,23 @@
   </sheetPr>
   <dimension ref="A1:Q343"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A316" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G328" activeCellId="0" sqref="G328"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="51" width="45.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="52" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="53" width="8.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="54" width="5.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="54" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="54" width="6.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="55" width="7.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="54" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="56" width="9.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="57" width="6.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="52" width="57.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="54" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="57" width="6.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="52" width="57.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="54" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="61" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3815,7 +3911,7 @@
       <c r="P2" s="69"/>
       <c r="Q2" s="69"/>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="71" t="s">
         <v>93</v>
       </c>
@@ -3849,6 +3945,9 @@
       <c r="I4" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J4" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="78" t="s">
@@ -3871,6 +3970,9 @@
       <c r="I5" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J5" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="78" t="s">
@@ -3999,10 +4101,13 @@
       <c r="I11" s="57" t="n">
         <v>2</v>
       </c>
+      <c r="J11" s="52" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="51" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F12" s="55" t="s">
         <v>22</v>
@@ -4017,10 +4122,13 @@
       <c r="I12" s="57" t="n">
         <v>1</v>
       </c>
+      <c r="J12" s="52" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="51" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F13" s="55" t="s">
         <v>22</v>
@@ -4035,10 +4143,13 @@
       <c r="I13" s="57" t="n">
         <v>6</v>
       </c>
+      <c r="J13" s="52" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F14" s="55" t="s">
         <v>22</v>
@@ -4053,10 +4164,13 @@
       <c r="I14" s="57" t="n">
         <v>5</v>
       </c>
+      <c r="J14" s="52" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="51" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F15" s="55" t="s">
         <v>22</v>
@@ -4071,10 +4185,13 @@
       <c r="I15" s="57" t="n">
         <v>2</v>
       </c>
+      <c r="J15" s="52" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F16" s="55" t="s">
         <v>22</v>
@@ -4092,7 +4209,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F17" s="55" t="s">
         <v>22</v>
@@ -4107,10 +4224,13 @@
       <c r="I17" s="57" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F18" s="55" t="s">
         <v>22</v>
@@ -4125,11 +4245,13 @@
       <c r="I18" s="57" t="n">
         <v>35</v>
       </c>
-      <c r="J18" s="86"/>
+      <c r="J18" s="52" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F19" s="55" t="s">
         <v>22</v>
@@ -4147,7 +4269,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F20" s="55" t="s">
         <v>22</v>
@@ -4165,7 +4287,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F21" s="55" t="s">
         <v>22</v>
@@ -4183,13 +4305,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F22" s="55" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H22" s="56" t="n">
         <f aca="false">H21+I21</f>
@@ -4198,16 +4320,19 @@
       <c r="I22" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J22" s="52" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F23" s="55" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H23" s="56" t="n">
         <f aca="false">H22+I22</f>
@@ -4219,7 +4344,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="51" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="F24" s="55" t="s">
         <v>22</v>
@@ -4237,13 +4362,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="51" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="F25" s="55" t="s">
         <v>22</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H25" s="56" t="n">
         <f aca="false">H24+I24</f>
@@ -4255,7 +4380,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="51" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F26" s="55" t="s">
         <v>22</v>
@@ -4270,10 +4395,13 @@
       <c r="I26" s="57" t="n">
         <v>10</v>
       </c>
+      <c r="J26" s="52" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="51" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="F27" s="55" t="s">
         <v>22</v>
@@ -4288,10 +4416,13 @@
       <c r="I27" s="57" t="n">
         <v>10</v>
       </c>
+      <c r="J27" s="52" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F28" s="55" t="s">
         <v>22</v>
@@ -4306,11 +4437,14 @@
       <c r="I28" s="57" t="n">
         <v>10</v>
       </c>
+      <c r="J28" s="52" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="71" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B30" s="72"/>
       <c r="C30" s="73"/>
@@ -4320,7 +4454,6 @@
       <c r="G30" s="74"/>
       <c r="H30" s="76"/>
       <c r="I30" s="77"/>
-      <c r="J30" s="86"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="78" t="s">
@@ -4331,7 +4464,7 @@
       <c r="D31" s="81"/>
       <c r="E31" s="81"/>
       <c r="F31" s="82" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="G31" s="83" t="s">
         <v>95</v>
@@ -4341,6 +4474,9 @@
       </c>
       <c r="I31" s="85" t="n">
         <v>25</v>
+      </c>
+      <c r="J31" s="52" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,7 +4488,7 @@
       <c r="D32" s="81"/>
       <c r="E32" s="81"/>
       <c r="F32" s="82" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="G32" s="81" t="s">
         <v>95</v>
@@ -4363,6 +4499,9 @@
       </c>
       <c r="I32" s="85" t="n">
         <v>22</v>
+      </c>
+      <c r="J32" s="52" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,7 +4513,7 @@
       <c r="D33" s="81"/>
       <c r="E33" s="81"/>
       <c r="F33" s="82" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="G33" s="81" t="s">
         <v>95</v>
@@ -4396,7 +4535,7 @@
       <c r="D34" s="81"/>
       <c r="E34" s="81"/>
       <c r="F34" s="82" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="G34" s="81" t="s">
         <v>95</v>
@@ -4418,7 +4557,7 @@
       <c r="D35" s="81"/>
       <c r="E35" s="81"/>
       <c r="F35" s="82" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="G35" s="81" t="s">
         <v>95</v>
@@ -4430,7 +4569,6 @@
       <c r="I35" s="85" t="n">
         <v>4</v>
       </c>
-      <c r="J35" s="86"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="78" t="s">
@@ -4441,7 +4579,7 @@
       <c r="D36" s="81"/>
       <c r="E36" s="81"/>
       <c r="F36" s="82" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="G36" s="81" t="s">
         <v>95</v>
@@ -4453,7 +4591,6 @@
       <c r="I36" s="85" t="n">
         <v>2</v>
       </c>
-      <c r="J36" s="86"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="78" t="s">
@@ -4464,7 +4601,7 @@
       <c r="D37" s="81"/>
       <c r="E37" s="81"/>
       <c r="F37" s="82" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="G37" s="81" t="s">
         <v>95</v>
@@ -4476,14 +4613,13 @@
       <c r="I37" s="85" t="n">
         <v>3</v>
       </c>
-      <c r="J37" s="86"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="51" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="F38" s="55" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H38" s="54" t="n">
         <v>101</v>
@@ -4491,59 +4627,64 @@
       <c r="I38" s="57" t="n">
         <v>30</v>
       </c>
-      <c r="J38" s="86"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="51" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="F39" s="55" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H39" s="54" t="n">
         <v>131</v>
       </c>
-      <c r="I39" s="87" t="n">
+      <c r="I39" s="86" t="n">
         <v>80</v>
       </c>
-      <c r="J39" s="88"/>
+      <c r="J39" s="87" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="51" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F40" s="55" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H40" s="54" t="n">
         <v>211</v>
       </c>
-      <c r="I40" s="87" t="n">
+      <c r="I40" s="86" t="n">
         <v>80</v>
       </c>
-      <c r="J40" s="88"/>
+      <c r="J40" s="87" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="51" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="F41" s="55" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H41" s="54" t="n">
         <v>291</v>
       </c>
-      <c r="I41" s="87" t="n">
+      <c r="I41" s="86" t="n">
         <v>80</v>
       </c>
-      <c r="J41" s="88"/>
+      <c r="J41" s="87" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="51" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="F42" s="55" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H42" s="54" t="n">
         <v>371</v>
@@ -4551,16 +4692,13 @@
       <c r="I42" s="57" t="n">
         <v>80</v>
       </c>
-      <c r="J42" s="86"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J43" s="86"/>
-    </row>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="71" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B46" s="72"/>
       <c r="C46" s="73"/>
@@ -4592,6 +4730,9 @@
       <c r="I47" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J47" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="78" t="s">
@@ -4614,6 +4755,9 @@
       <c r="I48" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J48" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="78" t="s">
@@ -4727,7 +4871,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="51" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="F54" s="55" t="n">
         <v>1000</v>
@@ -4745,7 +4889,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="51" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F55" s="55" t="n">
         <v>1000</v>
@@ -4763,7 +4907,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="51" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="F56" s="55" t="n">
         <v>1000</v>
@@ -4778,10 +4922,13 @@
       <c r="I56" s="57" t="n">
         <v>10</v>
       </c>
+      <c r="J56" s="52" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="51" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="F57" s="55" t="n">
         <v>1000</v>
@@ -4799,7 +4946,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="51" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="F58" s="55" t="n">
         <v>1000</v>
@@ -4814,16 +4961,19 @@
       <c r="I58" s="57" t="n">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J58" s="52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="51" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="F59" s="55" t="n">
         <v>1000</v>
       </c>
       <c r="G59" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H59" s="56" t="n">
         <f aca="false">H58+I58</f>
@@ -4832,16 +4982,19 @@
       <c r="I59" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J59" s="52" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="51" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="F60" s="55" t="n">
         <v>1000</v>
       </c>
       <c r="G60" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H60" s="56" t="n">
         <f aca="false">H59+I59</f>
@@ -4853,7 +5006,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="51" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="F61" s="55" t="n">
         <v>1000</v>
@@ -4868,10 +5021,13 @@
       <c r="I61" s="57" t="n">
         <v>30</v>
       </c>
+      <c r="J61" s="52" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="51" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="F62" s="55" t="n">
         <v>1000</v>
@@ -4889,7 +5045,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="51" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="F63" s="55" t="n">
         <v>1000</v>
@@ -4907,7 +5063,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="51" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="F64" s="55" t="n">
         <v>1000</v>
@@ -4925,7 +5081,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="51" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="F65" s="55" t="n">
         <v>1000</v>
@@ -4943,7 +5099,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="51" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="F66" s="55" t="n">
         <v>1000</v>
@@ -4961,7 +5117,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="51" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="F67" s="55" t="n">
         <v>1000</v>
@@ -4979,7 +5135,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="51" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F68" s="55" t="n">
         <v>1000</v>
@@ -4997,7 +5153,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="51" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="F69" s="55" t="n">
         <v>1000</v>
@@ -5015,13 +5171,13 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="51" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="F70" s="55" t="n">
         <v>1000</v>
       </c>
       <c r="G70" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H70" s="56" t="n">
         <f aca="false">H69+I69</f>
@@ -5033,7 +5189,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="51" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="F71" s="55" t="n">
         <v>1000</v>
@@ -5046,12 +5202,15 @@
       </c>
       <c r="I71" s="57" t="n">
         <v>1</v>
+      </c>
+      <c r="J71" s="52" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="71" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B73" s="72"/>
       <c r="C73" s="73"/>
@@ -5083,6 +5242,9 @@
       <c r="I74" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J74" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="78" t="s">
@@ -5105,6 +5267,9 @@
       <c r="I75" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J75" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="78" t="s">
@@ -5218,7 +5383,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="51" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="F81" s="55" t="n">
         <v>1060</v>
@@ -5236,7 +5401,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="51" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F82" s="55" t="n">
         <v>1060</v>
@@ -5254,13 +5419,13 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="51" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="F83" s="55" t="n">
         <v>1060</v>
       </c>
       <c r="G83" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H83" s="56" t="n">
         <f aca="false">H82+I82</f>
@@ -5272,13 +5437,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="51" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="F84" s="55" t="n">
         <v>1060</v>
       </c>
       <c r="G84" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H84" s="56" t="n">
         <f aca="false">H83+I83</f>
@@ -5290,7 +5455,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="51" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="F85" s="55" t="n">
         <v>1060</v>
@@ -5308,7 +5473,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="51" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="F86" s="55" t="n">
         <v>1060</v>
@@ -5326,7 +5491,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="51" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="F87" s="55" t="n">
         <v>1060</v>
@@ -5344,13 +5509,13 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="51" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="F88" s="55" t="n">
         <v>1060</v>
       </c>
       <c r="G88" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H88" s="56" t="n">
         <f aca="false">H87+I87</f>
@@ -5362,7 +5527,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="51" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="F89" s="55" t="n">
         <v>1060</v>
@@ -5380,7 +5545,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="51" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="F90" s="55" t="n">
         <v>1060</v>
@@ -5398,7 +5563,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="51" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="F91" s="55" t="n">
         <v>1060</v>
@@ -5416,7 +5581,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="51" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="F92" s="55" t="n">
         <v>1060</v>
@@ -5434,7 +5599,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="51" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="F93" s="55" t="n">
         <v>1060</v>
@@ -5452,13 +5617,13 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="51" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="F94" s="55" t="n">
         <v>1060</v>
       </c>
       <c r="G94" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H94" s="56" t="n">
         <f aca="false">H93+I93</f>
@@ -5470,13 +5635,13 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="51" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="F95" s="55" t="n">
         <v>1060</v>
       </c>
       <c r="G95" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H95" s="56" t="n">
         <f aca="false">H94+I94</f>
@@ -5488,7 +5653,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="51" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="F96" s="55" t="n">
         <v>1060</v>
@@ -5506,7 +5671,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="51" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="F97" s="55" t="n">
         <v>1060</v>
@@ -5525,7 +5690,7 @@
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="71" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="B99" s="72"/>
       <c r="C99" s="73"/>
@@ -5535,7 +5700,9 @@
       <c r="G99" s="74"/>
       <c r="H99" s="76"/>
       <c r="I99" s="77"/>
-      <c r="J99" s="72"/>
+      <c r="J99" s="72" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="78" t="s">
@@ -5557,6 +5724,9 @@
       <c r="I100" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J100" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="78" t="s">
@@ -5579,6 +5749,9 @@
       <c r="I101" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J101" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="78" t="s">
@@ -5692,7 +5865,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="51" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="F107" s="55" t="n">
         <v>1070</v>
@@ -5707,10 +5880,13 @@
       <c r="I107" s="57" t="n">
         <v>30</v>
       </c>
+      <c r="J107" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="51" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="F108" s="55" t="n">
         <v>1070</v>
@@ -5728,7 +5904,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="51" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="F109" s="55" t="n">
         <v>1070</v>
@@ -5746,7 +5922,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="51" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="F110" s="55" t="n">
         <v>1070</v>
@@ -5764,7 +5940,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="51" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="F111" s="55" t="n">
         <v>1070</v>
@@ -5782,7 +5958,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="51" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="F112" s="55" t="n">
         <v>1070</v>
@@ -5800,7 +5976,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="51" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F113" s="55" t="n">
         <v>1070</v>
@@ -5818,7 +5994,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="51" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="F114" s="55" t="n">
         <v>1070</v>
@@ -5836,7 +6012,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="51" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="F115" s="55" t="n">
         <v>1070</v>
@@ -5854,7 +6030,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="51" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="F116" s="55" t="n">
         <v>1070</v>
@@ -5872,7 +6048,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="51" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="F117" s="55" t="n">
         <v>1070</v>
@@ -5890,7 +6066,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="51" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="F118" s="55" t="n">
         <v>1070</v>
@@ -5908,7 +6084,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="51" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="F119" s="55" t="n">
         <v>1070</v>
@@ -5926,7 +6102,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="51" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="F120" s="55" t="n">
         <v>1070</v>
@@ -5944,7 +6120,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="51" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="F121" s="55" t="n">
         <v>1070</v>
@@ -5962,7 +6138,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="51" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="F122" s="55" t="n">
         <v>1070</v>
@@ -5981,7 +6157,7 @@
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="71" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="B124" s="72"/>
       <c r="C124" s="73"/>
@@ -6013,6 +6189,9 @@
       <c r="I125" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J125" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="78" t="s">
@@ -6035,6 +6214,9 @@
       <c r="I126" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J126" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="78" t="s">
@@ -6146,56 +6328,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="89" t="s">
-        <v>185</v>
-      </c>
-      <c r="B132" s="90"/>
-      <c r="C132" s="89"/>
-      <c r="D132" s="91"/>
-      <c r="E132" s="91"/>
-      <c r="F132" s="92" t="n">
+    <row r="132" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="88" t="s">
+        <v>203</v>
+      </c>
+      <c r="B132" s="89"/>
+      <c r="C132" s="88"/>
+      <c r="D132" s="90"/>
+      <c r="E132" s="90"/>
+      <c r="F132" s="91" t="n">
         <v>1100</v>
       </c>
-      <c r="G132" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="H132" s="93" t="n">
+      <c r="G132" s="90" t="s">
+        <v>103</v>
+      </c>
+      <c r="H132" s="92" t="n">
         <f aca="false">H131+I131</f>
         <v>101</v>
       </c>
-      <c r="I132" s="91" t="n">
+      <c r="I132" s="90" t="n">
         <v>400</v>
       </c>
-      <c r="J132" s="90"/>
+      <c r="J132" s="89" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="89" t="s">
-        <v>186</v>
-      </c>
-      <c r="B133" s="90"/>
-      <c r="C133" s="89"/>
-      <c r="D133" s="91"/>
-      <c r="E133" s="91"/>
-      <c r="F133" s="92" t="n">
+      <c r="A133" s="88" t="s">
+        <v>205</v>
+      </c>
+      <c r="B133" s="89"/>
+      <c r="C133" s="88"/>
+      <c r="D133" s="90"/>
+      <c r="E133" s="90"/>
+      <c r="F133" s="91" t="n">
         <v>1100</v>
       </c>
-      <c r="G133" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="H133" s="93" t="n">
+      <c r="G133" s="90" t="s">
+        <v>103</v>
+      </c>
+      <c r="H133" s="92" t="n">
         <f aca="false">H132+I132</f>
         <v>501</v>
       </c>
-      <c r="I133" s="91" t="n">
+      <c r="I133" s="90" t="n">
         <v>400</v>
       </c>
-      <c r="J133" s="90"/>
+      <c r="J133" s="89" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="71" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="B135" s="72"/>
       <c r="C135" s="73"/>
@@ -6227,6 +6413,9 @@
       <c r="I136" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J136" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="78" t="s">
@@ -6249,6 +6438,9 @@
       <c r="I137" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J137" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="78" t="s">
@@ -6362,13 +6554,13 @@
     </row>
     <row r="143" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="51" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="F143" s="55" t="n">
         <v>1110</v>
       </c>
       <c r="G143" s="54" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H143" s="56" t="n">
         <f aca="false">H142+I142</f>
@@ -6377,6 +6569,9 @@
       <c r="I143" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J143" s="52" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F144" s="55" t="n">
@@ -6395,7 +6590,7 @@
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="71" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="B146" s="72"/>
       <c r="C146" s="73"/>
@@ -6427,6 +6622,9 @@
       <c r="I147" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J147" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="78" t="s">
@@ -6449,6 +6647,9 @@
       <c r="I148" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J148" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="78" t="s">
@@ -6562,7 +6763,7 @@
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="51" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="F154" s="55" t="n">
         <v>1200</v>
@@ -6570,16 +6771,19 @@
       <c r="G154" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H154" s="94" t="n">
+      <c r="H154" s="93" t="n">
         <v>101</v>
       </c>
       <c r="I154" s="57" t="n">
         <v>30</v>
       </c>
+      <c r="J154" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="95" t="s">
-        <v>192</v>
+      <c r="A155" s="94" t="s">
+        <v>213</v>
       </c>
       <c r="F155" s="55" t="n">
         <v>1200</v>
@@ -6587,16 +6791,19 @@
       <c r="G155" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H155" s="94" t="n">
+      <c r="H155" s="93" t="n">
         <v>131</v>
       </c>
       <c r="I155" s="57" t="n">
         <v>80</v>
       </c>
+      <c r="J155" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="95" t="s">
-        <v>193</v>
+      <c r="A156" s="94" t="s">
+        <v>214</v>
       </c>
       <c r="F156" s="55" t="n">
         <v>1200</v>
@@ -6604,7 +6811,7 @@
       <c r="G156" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H156" s="94" t="n">
+      <c r="H156" s="93" t="n">
         <v>211</v>
       </c>
       <c r="I156" s="57" t="n">
@@ -6612,8 +6819,8 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="95" t="s">
-        <v>194</v>
+      <c r="A157" s="94" t="s">
+        <v>215</v>
       </c>
       <c r="F157" s="55" t="n">
         <v>1200</v>
@@ -6621,7 +6828,7 @@
       <c r="G157" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H157" s="94" t="n">
+      <c r="H157" s="93" t="n">
         <v>291</v>
       </c>
       <c r="I157" s="57" t="n">
@@ -6629,34 +6836,34 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="96" t="s">
-        <v>195</v>
-      </c>
-      <c r="B158" s="97"/>
-      <c r="C158" s="98"/>
-      <c r="D158" s="99"/>
-      <c r="E158" s="99"/>
-      <c r="F158" s="100" t="n">
+      <c r="A158" s="95" t="s">
+        <v>216</v>
+      </c>
+      <c r="B158" s="96"/>
+      <c r="C158" s="97"/>
+      <c r="D158" s="98"/>
+      <c r="E158" s="98"/>
+      <c r="F158" s="99" t="n">
         <v>1200</v>
       </c>
-      <c r="G158" s="99" t="s">
-        <v>103</v>
-      </c>
-      <c r="H158" s="101" t="n">
+      <c r="G158" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="H158" s="100" t="n">
         <v>371</v>
       </c>
-      <c r="I158" s="102" t="n">
+      <c r="I158" s="101" t="n">
         <v>80</v>
       </c>
-      <c r="J158" s="97"/>
+      <c r="J158" s="96"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="95"/>
-      <c r="H159" s="94"/>
+      <c r="A159" s="94"/>
+      <c r="H159" s="93"/>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="71" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="B160" s="72"/>
       <c r="C160" s="73"/>
@@ -6688,6 +6895,9 @@
       <c r="I161" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J161" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="78" t="s">
@@ -6710,6 +6920,9 @@
       <c r="I162" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J162" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="78" t="s">
@@ -6823,7 +7036,7 @@
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="51" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="F168" s="55" t="n">
         <v>1210</v>
@@ -6831,38 +7044,39 @@
       <c r="G168" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H168" s="94" t="n">
+      <c r="H168" s="93" t="n">
         <v>101</v>
       </c>
       <c r="I168" s="57" t="n">
         <v>30</v>
       </c>
+      <c r="J168" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="126" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="95" t="s">
-        <v>197</v>
-      </c>
-      <c r="B169" s="86"/>
-      <c r="C169" s="103"/>
-      <c r="D169" s="104"/>
-      <c r="E169" s="104"/>
-      <c r="F169" s="105" t="n">
+      <c r="A169" s="94" t="s">
+        <v>218</v>
+      </c>
+      <c r="F169" s="55" t="n">
         <v>1210</v>
       </c>
-      <c r="G169" s="104" t="s">
-        <v>103</v>
-      </c>
-      <c r="H169" s="106" t="n">
+      <c r="G169" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H169" s="102" t="n">
         <v>131</v>
       </c>
-      <c r="I169" s="107" t="n">
+      <c r="I169" s="57" t="n">
         <v>80</v>
       </c>
-      <c r="J169" s="86"/>
+      <c r="J169" s="52" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="95" t="s">
-        <v>198</v>
+      <c r="A170" s="94" t="s">
+        <v>220</v>
       </c>
       <c r="F170" s="55" t="n">
         <v>1210</v>
@@ -6870,16 +7084,19 @@
       <c r="G170" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H170" s="94" t="n">
+      <c r="H170" s="93" t="n">
         <v>211</v>
       </c>
       <c r="I170" s="57" t="n">
         <v>80</v>
       </c>
+      <c r="J170" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="95" t="s">
-        <v>199</v>
+      <c r="A171" s="94" t="s">
+        <v>221</v>
       </c>
       <c r="F171" s="55" t="n">
         <v>1210</v>
@@ -6887,16 +7104,19 @@
       <c r="G171" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H171" s="94" t="n">
+      <c r="H171" s="93" t="n">
         <v>291</v>
       </c>
       <c r="I171" s="57" t="n">
         <v>80</v>
       </c>
+      <c r="J171" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="95" t="s">
-        <v>200</v>
+      <c r="A172" s="94" t="s">
+        <v>222</v>
       </c>
       <c r="F172" s="55" t="n">
         <v>1210</v>
@@ -6904,16 +7124,19 @@
       <c r="G172" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H172" s="94" t="n">
+      <c r="H172" s="93" t="n">
         <v>371</v>
       </c>
       <c r="I172" s="57" t="n">
         <v>80</v>
       </c>
+      <c r="J172" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="95" t="s">
-        <v>201</v>
+      <c r="A173" s="94" t="s">
+        <v>223</v>
       </c>
       <c r="F173" s="55" t="n">
         <v>1210</v>
@@ -6924,15 +7147,17 @@
       <c r="H173" s="54" t="n">
         <v>421</v>
       </c>
-      <c r="I173" s="108" t="n">
+      <c r="I173" s="103" t="n">
         <v>80</v>
       </c>
-      <c r="J173" s="54"/>
+      <c r="J173" s="54" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="71" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="B175" s="72"/>
       <c r="C175" s="73"/>
@@ -6964,6 +7189,9 @@
       <c r="I176" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J176" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="78" t="s">
@@ -6986,6 +7214,9 @@
       <c r="I177" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J177" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="78" t="s">
@@ -7099,7 +7330,7 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="51" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="F183" s="55" t="n">
         <v>1400</v>
@@ -7116,7 +7347,7 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="51" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="F184" s="55" t="n">
         <v>1400</v>
@@ -7130,10 +7361,13 @@
       <c r="I184" s="57" t="n">
         <v>35</v>
       </c>
+      <c r="J184" s="52" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="51" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="F185" s="55" t="n">
         <v>1400</v>
@@ -7148,10 +7382,13 @@
       <c r="I185" s="57" t="n">
         <v>60</v>
       </c>
+      <c r="J185" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="51" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="F186" s="55" t="n">
         <v>1400</v>
@@ -7169,7 +7406,7 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="51" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="F187" s="55" t="n">
         <v>1400</v>
@@ -7187,7 +7424,7 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="51" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="F188" s="55" t="n">
         <v>1400</v>
@@ -7205,7 +7442,7 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="51" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="F189" s="55" t="n">
         <v>1400</v>
@@ -7223,7 +7460,7 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="51" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="F190" s="55" t="n">
         <v>1400</v>
@@ -7241,7 +7478,7 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="51" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="F191" s="55" t="n">
         <v>1400</v>
@@ -7259,7 +7496,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="51" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="F192" s="55" t="n">
         <v>1400</v>
@@ -7277,7 +7514,7 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="51" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="F193" s="55" t="n">
         <v>1400</v>
@@ -7295,7 +7532,7 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="51" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="F194" s="55" t="n">
         <v>1400</v>
@@ -7313,7 +7550,7 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="51" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="F195" s="55" t="n">
         <v>1400</v>
@@ -7331,7 +7568,7 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="51" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="F196" s="55" t="n">
         <v>1400</v>
@@ -7349,7 +7586,7 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="51" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="F197" s="55" t="n">
         <v>1400</v>
@@ -7367,7 +7604,7 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="51" t="s">
-        <v>218</v>
+        <v>241</v>
       </c>
       <c r="F198" s="55" t="n">
         <v>1400</v>
@@ -7385,7 +7622,7 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="51" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="F199" s="55" t="n">
         <v>1400</v>
@@ -7404,7 +7641,7 @@
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="71" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="B201" s="72"/>
       <c r="C201" s="73"/>
@@ -7436,6 +7673,9 @@
       <c r="I202" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J202" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="78" t="s">
@@ -7458,6 +7698,9 @@
       <c r="I203" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J203" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="78" t="s">
@@ -7571,7 +7814,7 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="51" t="s">
-        <v>221</v>
+        <v>244</v>
       </c>
       <c r="F209" s="55" t="n">
         <v>1500</v>
@@ -7587,32 +7830,30 @@
         <v>60</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="B210" s="86"/>
-      <c r="C210" s="103"/>
-      <c r="D210" s="104"/>
-      <c r="E210" s="104"/>
-      <c r="F210" s="105" t="n">
+        <v>245</v>
+      </c>
+      <c r="F210" s="55" t="n">
         <v>1500</v>
       </c>
-      <c r="G210" s="104" t="s">
-        <v>103</v>
-      </c>
-      <c r="H210" s="109" t="n">
+      <c r="G210" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H210" s="104" t="n">
         <f aca="false">H209+I209</f>
         <v>161</v>
       </c>
-      <c r="I210" s="107" t="n">
+      <c r="I210" s="57" t="n">
         <v>35</v>
       </c>
-      <c r="J210" s="86"/>
+      <c r="J210" s="52" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="51" t="s">
-        <v>223</v>
+        <v>246</v>
       </c>
       <c r="F211" s="55" t="n">
         <v>1500</v>
@@ -7627,10 +7868,13 @@
       <c r="I211" s="57" t="n">
         <v>60</v>
       </c>
+      <c r="J211" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="51" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="F212" s="55" t="n">
         <v>1500</v>
@@ -7645,10 +7889,13 @@
       <c r="I212" s="57" t="n">
         <v>35</v>
       </c>
+      <c r="J212" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="51" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="F213" s="55" t="n">
         <v>1500</v>
@@ -7666,7 +7913,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="51" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="F214" s="55" t="n">
         <v>1500</v>
@@ -7684,7 +7931,7 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="F215" s="55" t="n">
         <v>1500</v>
@@ -7702,7 +7949,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="51" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="F216" s="55" t="n">
         <v>1500</v>
@@ -7717,10 +7964,13 @@
       <c r="I216" s="57" t="n">
         <v>30</v>
       </c>
+      <c r="J216" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="51" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="F217" s="55" t="n">
         <v>1500</v>
@@ -7735,10 +7985,13 @@
       <c r="I217" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J217" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="51" t="s">
-        <v>230</v>
+        <v>253</v>
       </c>
       <c r="F218" s="55" t="n">
         <v>1500</v>
@@ -7756,7 +8009,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="51" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="F219" s="55" t="n">
         <v>1500</v>
@@ -7774,7 +8027,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="51" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="F220" s="55" t="n">
         <v>1500</v>
@@ -7789,10 +8042,13 @@
       <c r="I220" s="57" t="n">
         <v>20</v>
       </c>
+      <c r="J220" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="51" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="F221" s="55" t="n">
         <v>1500</v>
@@ -7810,7 +8066,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="51" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="F222" s="55" t="n">
         <v>1500</v>
@@ -7828,7 +8084,7 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="51" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
       <c r="F223" s="55" t="n">
         <v>1500</v>
@@ -7846,7 +8102,7 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="51" t="s">
-        <v>236</v>
+        <v>259</v>
       </c>
       <c r="F224" s="55" t="n">
         <v>1500</v>
@@ -7864,7 +8120,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="51" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="F225" s="55" t="n">
         <v>1500</v>
@@ -7881,33 +8137,33 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="227" s="112" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" s="107" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="71" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="B227" s="52"/>
       <c r="C227" s="52"/>
-      <c r="D227" s="110"/>
-      <c r="E227" s="110"/>
-      <c r="F227" s="111"/>
-      <c r="H227" s="113"/>
-      <c r="I227" s="114"/>
+      <c r="D227" s="105"/>
+      <c r="E227" s="105"/>
+      <c r="F227" s="106"/>
+      <c r="H227" s="108"/>
+      <c r="I227" s="109"/>
       <c r="J227" s="52"/>
     </row>
-    <row r="228" s="112" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" s="107" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="51"/>
       <c r="B228" s="52"/>
       <c r="C228" s="52"/>
-      <c r="D228" s="110"/>
-      <c r="E228" s="110"/>
-      <c r="F228" s="111"/>
-      <c r="H228" s="113"/>
-      <c r="I228" s="114"/>
+      <c r="D228" s="105"/>
+      <c r="E228" s="105"/>
+      <c r="F228" s="106"/>
+      <c r="H228" s="108"/>
+      <c r="I228" s="109"/>
       <c r="J228" s="52"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="71" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="B229" s="72"/>
       <c r="C229" s="73"/>
@@ -7939,6 +8195,9 @@
       <c r="I230" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J230" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="78" t="s">
@@ -7961,6 +8220,9 @@
       <c r="I231" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J231" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="78" t="s">
@@ -7983,6 +8245,9 @@
       <c r="I232" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J232" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="78" t="s">
@@ -8005,6 +8270,9 @@
       <c r="I233" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J233" s="52" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="78" t="s">
@@ -8074,7 +8342,7 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="51" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="F237" s="55" t="n">
         <v>2000</v>
@@ -8089,16 +8357,19 @@
       <c r="I237" s="57" t="n">
         <v>20</v>
       </c>
+      <c r="J237" s="52" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="51" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="F238" s="55" t="n">
         <v>2000</v>
       </c>
       <c r="G238" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H238" s="56" t="n">
         <f aca="false">H237+I237</f>
@@ -8107,10 +8378,13 @@
       <c r="I238" s="57" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J238" s="52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="51" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="F239" s="55" t="n">
         <v>2000</v>
@@ -8125,10 +8399,13 @@
       <c r="I239" s="57" t="n">
         <v>50</v>
       </c>
+      <c r="J239" s="52" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="51" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="F240" s="55" t="n">
         <v>2000</v>
@@ -8144,9 +8421,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="51" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="F241" s="55" t="n">
         <v>2000</v>
@@ -8161,11 +8438,13 @@
       <c r="I241" s="57" t="n">
         <v>50</v>
       </c>
-      <c r="J241" s="112"/>
+      <c r="J241" s="107" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="51" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="F242" s="55" t="n">
         <v>2000</v>
@@ -8183,7 +8462,7 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="51" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="F243" s="55" t="n">
         <v>2000</v>
@@ -8201,7 +8480,7 @@
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="51" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="F244" s="55" t="n">
         <v>2000</v>
@@ -8217,9 +8496,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="51" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="F245" s="55" t="n">
         <v>2000</v>
@@ -8234,10 +8513,13 @@
       <c r="I245" s="57" t="n">
         <v>50</v>
       </c>
+      <c r="J245" s="52" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="51" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="F246" s="55" t="n">
         <v>2000</v>
@@ -8252,10 +8534,13 @@
       <c r="I246" s="57" t="n">
         <v>50</v>
       </c>
+      <c r="J246" s="52" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="51" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="F247" s="55" t="n">
         <v>2000</v>
@@ -8273,7 +8558,7 @@
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="51" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="F248" s="55" t="n">
         <v>2000</v>
@@ -8291,7 +8576,7 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="51" t="s">
-        <v>252</v>
+        <v>281</v>
       </c>
       <c r="F249" s="55" t="n">
         <v>2000</v>
@@ -8309,13 +8594,13 @@
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="51" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="F250" s="55" t="n">
         <v>2000</v>
       </c>
       <c r="G250" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H250" s="56" t="n">
         <f aca="false">H249+I249</f>
@@ -8328,7 +8613,7 @@
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="71" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="B252" s="72"/>
       <c r="C252" s="73"/>
@@ -8360,6 +8645,9 @@
       <c r="I253" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J253" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="78" t="s">
@@ -8382,6 +8670,9 @@
       <c r="I254" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J254" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="78" t="s">
@@ -8404,6 +8695,9 @@
       <c r="I255" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J255" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="78" t="s">
@@ -8426,6 +8720,9 @@
       <c r="I256" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J256" s="52" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="78" t="s">
@@ -8495,7 +8792,7 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="51" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="F260" s="55" t="n">
         <v>3000</v>
@@ -8510,16 +8807,19 @@
       <c r="I260" s="57" t="n">
         <v>1</v>
       </c>
+      <c r="J260" s="52" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="51" t="s">
-        <v>255</v>
+        <v>285</v>
       </c>
       <c r="F261" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G261" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H261" s="56" t="n">
         <f aca="false">H260+I260</f>
@@ -8528,10 +8828,13 @@
       <c r="I261" s="57" t="n">
         <v>22</v>
       </c>
+      <c r="J261" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="51" t="s">
-        <v>256</v>
+        <v>286</v>
       </c>
       <c r="F262" s="55" t="n">
         <v>3000</v>
@@ -8546,10 +8849,13 @@
       <c r="I262" s="57" t="n">
         <v>3</v>
       </c>
+      <c r="J262" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="51" t="s">
-        <v>257</v>
+        <v>287</v>
       </c>
       <c r="F263" s="55" t="n">
         <v>3000</v>
@@ -8564,16 +8870,19 @@
       <c r="I263" s="57" t="n">
         <v>10</v>
       </c>
+      <c r="J263" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="51" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="F264" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G264" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H264" s="56" t="n">
         <f aca="false">H263+I263</f>
@@ -8585,13 +8894,13 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="51" t="s">
-        <v>259</v>
+        <v>289</v>
       </c>
       <c r="F265" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G265" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H265" s="56" t="n">
         <f aca="false">H264+I264</f>
@@ -8603,13 +8912,13 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="51" t="s">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="F266" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G266" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H266" s="56" t="n">
         <f aca="false">H265+I265</f>
@@ -8621,13 +8930,13 @@
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="51" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="F267" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G267" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H267" s="56" t="n">
         <f aca="false">H266+I266</f>
@@ -8639,13 +8948,13 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="51" t="s">
-        <v>262</v>
+        <v>292</v>
       </c>
       <c r="F268" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G268" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H268" s="56" t="n">
         <f aca="false">H267+I267</f>
@@ -8657,13 +8966,13 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="51" t="s">
-        <v>263</v>
+        <v>293</v>
       </c>
       <c r="F269" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G269" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H269" s="56" t="n">
         <f aca="false">H268+I268</f>
@@ -8675,13 +8984,13 @@
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="51" t="s">
-        <v>264</v>
+        <v>294</v>
       </c>
       <c r="F270" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G270" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H270" s="56" t="n">
         <f aca="false">H269+I269</f>
@@ -8693,7 +9002,7 @@
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="51" t="s">
-        <v>265</v>
+        <v>295</v>
       </c>
       <c r="F271" s="55" t="n">
         <v>3000</v>
@@ -8711,7 +9020,7 @@
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="51" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="F272" s="55" t="n">
         <v>3000</v>
@@ -8729,7 +9038,7 @@
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="51" t="s">
-        <v>266</v>
+        <v>296</v>
       </c>
       <c r="F273" s="55" t="n">
         <v>3000</v>
@@ -8747,7 +9056,7 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="51" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
       <c r="F274" s="55" t="n">
         <v>3000</v>
@@ -8765,7 +9074,7 @@
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="51" t="s">
-        <v>268</v>
+        <v>298</v>
       </c>
       <c r="F275" s="55" t="n">
         <v>3000</v>
@@ -8783,7 +9092,7 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="51" t="s">
-        <v>269</v>
+        <v>299</v>
       </c>
       <c r="F276" s="55" t="n">
         <v>3000</v>
@@ -8801,7 +9110,7 @@
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="51" t="s">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="F277" s="55" t="n">
         <v>3000</v>
@@ -8819,7 +9128,7 @@
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="51" t="s">
-        <v>271</v>
+        <v>301</v>
       </c>
       <c r="F278" s="55" t="n">
         <v>3000</v>
@@ -8837,13 +9146,13 @@
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="51" t="s">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="F279" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G279" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H279" s="56" t="n">
         <f aca="false">H278+I278</f>
@@ -8855,13 +9164,13 @@
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="51" t="s">
-        <v>273</v>
+        <v>303</v>
       </c>
       <c r="F280" s="55" t="n">
         <v>3000</v>
       </c>
       <c r="G280" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H280" s="56" t="n">
         <f aca="false">H279+I279</f>
@@ -8873,7 +9182,7 @@
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="51" t="s">
-        <v>274</v>
+        <v>304</v>
       </c>
       <c r="F281" s="55" t="n">
         <v>3000</v>
@@ -8891,7 +9200,7 @@
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="51" t="s">
-        <v>275</v>
+        <v>305</v>
       </c>
       <c r="F282" s="55" t="n">
         <v>3000</v>
@@ -8910,7 +9219,7 @@
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="71" t="s">
-        <v>276</v>
+        <v>306</v>
       </c>
       <c r="B284" s="72"/>
       <c r="C284" s="73"/>
@@ -8942,6 +9251,9 @@
       <c r="I285" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J285" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="78" t="s">
@@ -8964,6 +9276,9 @@
       <c r="I286" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J286" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="78" t="s">
@@ -8986,6 +9301,9 @@
       <c r="I287" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J287" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="78" t="s">
@@ -9008,6 +9326,9 @@
       <c r="I288" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J288" s="52" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="78" t="s">
@@ -9077,7 +9398,7 @@
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="51" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
       <c r="F292" s="55" t="n">
         <v>4000</v>
@@ -9095,7 +9416,7 @@
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="51" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
       <c r="F293" s="55" t="n">
         <v>4000</v>
@@ -9113,13 +9434,13 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="51" t="s">
-        <v>279</v>
+        <v>309</v>
       </c>
       <c r="F294" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G294" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H294" s="56" t="n">
         <f aca="false">H293+I293</f>
@@ -9128,10 +9449,13 @@
       <c r="I294" s="57" t="n">
         <v>22</v>
       </c>
+      <c r="J294" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="51" t="s">
-        <v>280</v>
+        <v>310</v>
       </c>
       <c r="F295" s="55" t="n">
         <v>4000</v>
@@ -9146,10 +9470,13 @@
       <c r="I295" s="57" t="n">
         <v>10</v>
       </c>
+      <c r="J295" s="52" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="51" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
       <c r="F296" s="55" t="n">
         <v>4000</v>
@@ -9165,15 +9492,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="51" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="F297" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G297" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H297" s="56" t="n">
         <f aca="false">H296+I296</f>
@@ -9182,16 +9509,19 @@
       <c r="I297" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J297" s="52" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="51" t="s">
-        <v>283</v>
+        <v>315</v>
       </c>
       <c r="F298" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G298" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H298" s="56" t="n">
         <f aca="false">H297+I297</f>
@@ -9203,13 +9533,13 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="51" t="s">
-        <v>284</v>
+        <v>316</v>
       </c>
       <c r="F299" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G299" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H299" s="56" t="n">
         <f aca="false">H298+I298</f>
@@ -9221,13 +9551,13 @@
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="51" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
       <c r="F300" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G300" s="54" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H300" s="56" t="n">
         <f aca="false">H299+I299</f>
@@ -9236,16 +9566,19 @@
       <c r="I300" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J300" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="51" t="s">
-        <v>286</v>
+        <v>318</v>
       </c>
       <c r="F301" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G301" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H301" s="56" t="n">
         <f aca="false">H300+I300</f>
@@ -9254,10 +9587,13 @@
       <c r="I301" s="57" t="n">
         <v>22</v>
       </c>
+      <c r="J301" s="52" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="51" t="s">
-        <v>287</v>
+        <v>320</v>
       </c>
       <c r="F302" s="55" t="n">
         <v>4000</v>
@@ -9272,10 +9608,13 @@
       <c r="I302" s="57" t="n">
         <v>3</v>
       </c>
+      <c r="J302" s="52" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="51" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="F303" s="55" t="n">
         <v>4000</v>
@@ -9293,13 +9632,13 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="51" t="s">
-        <v>289</v>
+        <v>323</v>
       </c>
       <c r="F304" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G304" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H304" s="56" t="n">
         <f aca="false">H303+I303</f>
@@ -9308,10 +9647,13 @@
       <c r="I304" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J304" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="51" t="s">
-        <v>290</v>
+        <v>324</v>
       </c>
       <c r="F305" s="55" t="n">
         <v>4000</v>
@@ -9329,7 +9671,7 @@
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="51" t="s">
-        <v>291</v>
+        <v>325</v>
       </c>
       <c r="F306" s="55" t="n">
         <v>4000</v>
@@ -9344,16 +9686,19 @@
       <c r="I306" s="57" t="n">
         <v>10</v>
       </c>
+      <c r="J306" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="51" t="s">
-        <v>292</v>
+        <v>326</v>
       </c>
       <c r="F307" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G307" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H307" s="56" t="n">
         <f aca="false">H306+I306</f>
@@ -9365,13 +9710,13 @@
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="51" t="s">
-        <v>293</v>
+        <v>327</v>
       </c>
       <c r="F308" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G308" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H308" s="56" t="n">
         <f aca="false">H307+I307</f>
@@ -9383,7 +9728,7 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="51" t="s">
-        <v>294</v>
+        <v>328</v>
       </c>
       <c r="F309" s="55" t="n">
         <v>4000</v>
@@ -9401,7 +9746,7 @@
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="51" t="s">
-        <v>295</v>
+        <v>329</v>
       </c>
       <c r="F310" s="55" t="n">
         <v>4000</v>
@@ -9419,7 +9764,7 @@
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="51" t="s">
-        <v>296</v>
+        <v>330</v>
       </c>
       <c r="F311" s="55" t="n">
         <v>4000</v>
@@ -9437,7 +9782,7 @@
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="51" t="s">
-        <v>297</v>
+        <v>331</v>
       </c>
       <c r="F312" s="55" t="n">
         <v>4000</v>
@@ -9455,7 +9800,7 @@
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="51" t="s">
-        <v>298</v>
+        <v>332</v>
       </c>
       <c r="F313" s="55" t="n">
         <v>4000</v>
@@ -9473,7 +9818,7 @@
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="51" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
       <c r="F314" s="55" t="n">
         <v>4000</v>
@@ -9491,7 +9836,7 @@
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="51" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="F315" s="55" t="n">
         <v>4000</v>
@@ -9509,13 +9854,13 @@
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="51" t="s">
-        <v>301</v>
+        <v>335</v>
       </c>
       <c r="F316" s="55" t="n">
         <v>4000</v>
       </c>
       <c r="G316" s="54" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H316" s="56" t="n">
         <v>537</v>
@@ -9528,7 +9873,7 @@
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="71" t="s">
-        <v>302</v>
+        <v>336</v>
       </c>
       <c r="B319" s="72"/>
       <c r="C319" s="73"/>
@@ -9560,6 +9905,9 @@
       <c r="I320" s="85" t="n">
         <v>25</v>
       </c>
+      <c r="J320" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="78" t="s">
@@ -9582,6 +9930,9 @@
       <c r="I321" s="85" t="n">
         <v>22</v>
       </c>
+      <c r="J321" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="78" t="s">
@@ -9695,7 +10046,7 @@
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="51" t="s">
-        <v>221</v>
+        <v>244</v>
       </c>
       <c r="F327" s="55" t="n">
         <v>4800</v>
@@ -9713,7 +10064,7 @@
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="51" t="s">
-        <v>222</v>
+        <v>245</v>
       </c>
       <c r="F328" s="55" t="n">
         <v>4800</v>
@@ -9728,10 +10079,16 @@
       <c r="I328" s="57" t="n">
         <v>35</v>
       </c>
+      <c r="J328" s="52" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="51" t="s">
-        <v>223</v>
+        <v>246</v>
+      </c>
+      <c r="B329" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="F329" s="55" t="n">
         <v>4800</v>
@@ -9746,10 +10103,16 @@
       <c r="I329" s="57" t="n">
         <v>60</v>
       </c>
+      <c r="J329" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="51" t="s">
-        <v>224</v>
+        <v>247</v>
+      </c>
+      <c r="B330" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="F330" s="55" t="n">
         <v>4800</v>
@@ -9764,10 +10127,16 @@
       <c r="I330" s="57" t="n">
         <v>35</v>
       </c>
+      <c r="J330" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="51" t="s">
-        <v>225</v>
+        <v>248</v>
+      </c>
+      <c r="B331" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="F331" s="55" t="n">
         <v>4800</v>
@@ -9785,7 +10154,7 @@
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="51" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="F332" s="55" t="n">
         <v>4800</v>
@@ -9803,7 +10172,7 @@
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="F333" s="55" t="n">
         <v>4800</v>
@@ -9821,7 +10190,10 @@
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="51" t="s">
-        <v>228</v>
+        <v>251</v>
+      </c>
+      <c r="B334" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="F334" s="55" t="n">
         <v>4800</v>
@@ -9836,10 +10208,16 @@
       <c r="I334" s="57" t="n">
         <v>30</v>
       </c>
+      <c r="J334" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="51" t="s">
-        <v>229</v>
+        <v>252</v>
+      </c>
+      <c r="B335" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="F335" s="55" t="n">
         <v>4800</v>
@@ -9854,10 +10232,16 @@
       <c r="I335" s="57" t="n">
         <v>15</v>
       </c>
+      <c r="J335" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="51" t="s">
-        <v>230</v>
+        <v>253</v>
+      </c>
+      <c r="B336" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="F336" s="55" t="n">
         <v>4800</v>
@@ -9875,7 +10259,7 @@
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="51" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="F337" s="55" t="n">
         <v>4800</v>
@@ -9893,7 +10277,10 @@
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="51" t="s">
-        <v>232</v>
+        <v>255</v>
+      </c>
+      <c r="B338" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="F338" s="55" t="n">
         <v>4800</v>
@@ -9908,10 +10295,13 @@
       <c r="I338" s="57" t="n">
         <v>20</v>
       </c>
+      <c r="J338" s="52" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="51" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="F339" s="55" t="n">
         <v>4800</v>
@@ -9929,7 +10319,7 @@
     </row>
     <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="51" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="F340" s="55" t="n">
         <v>4800</v>
@@ -9947,7 +10337,7 @@
     </row>
     <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="51" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
       <c r="F341" s="55" t="n">
         <v>4800</v>
@@ -9965,7 +10355,7 @@
     </row>
     <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="51" t="s">
-        <v>236</v>
+        <v>259</v>
       </c>
       <c r="F342" s="55" t="n">
         <v>4800</v>
@@ -9983,7 +10373,7 @@
     </row>
     <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="51" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="F343" s="55" t="n">
         <v>4800</v>
@@ -10036,76 +10426,76 @@
       <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>303</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>304</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>305</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>306</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>307</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>308</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>309</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>310</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>311</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>312</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>313</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>314</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>315</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -10130,156 +10520,156 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="115" t="s">
-        <v>317</v>
+      <c r="A2" s="110" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="115" t="s">
-        <v>318</v>
+      <c r="A3" s="110" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="115" t="s">
-        <v>319</v>
+      <c r="A4" s="110" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="115" t="s">
-        <v>320</v>
+      <c r="A5" s="110" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="115" t="s">
-        <v>321</v>
+      <c r="A6" s="110" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="115" t="s">
-        <v>322</v>
+      <c r="A7" s="110" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="115" t="s">
-        <v>323</v>
+      <c r="A8" s="110" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="115" t="s">
-        <v>324</v>
+      <c r="A9" s="110" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="115" t="s">
-        <v>325</v>
+      <c r="A10" s="110" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="115" t="s">
-        <v>326</v>
+      <c r="A11" s="110" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="115" t="s">
-        <v>327</v>
+      <c r="A12" s="110" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="115" t="s">
-        <v>328</v>
+      <c r="A13" s="110" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="115" t="s">
-        <v>329</v>
+      <c r="A14" s="110" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="115" t="s">
-        <v>330</v>
+      <c r="A15" s="110" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="115" t="s">
-        <v>331</v>
+      <c r="A16" s="110" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="115" t="s">
-        <v>332</v>
+      <c r="A17" s="110" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="115" t="s">
-        <v>333</v>
+      <c r="A18" s="110" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="115" t="s">
-        <v>334</v>
+      <c r="A19" s="110" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="115" t="s">
-        <v>335</v>
+      <c r="A20" s="110" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="115" t="s">
-        <v>336</v>
+      <c r="A21" s="110" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="115" t="s">
-        <v>337</v>
+      <c r="A22" s="110" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="115" t="s">
-        <v>338</v>
+      <c r="A23" s="110" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="115" t="s">
-        <v>339</v>
+      <c r="A24" s="110" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="115" t="s">
-        <v>340</v>
+      <c r="A25" s="110" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="115" t="s">
-        <v>341</v>
+      <c r="A26" s="110" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="115" t="s">
-        <v>342</v>
+      <c r="A27" s="110" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="115" t="s">
-        <v>343</v>
+      <c r="A28" s="110" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="115" t="s">
-        <v>344</v>
+      <c r="A29" s="110" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="115" t="s">
-        <v>345</v>
+      <c r="A30" s="110" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="115" t="s">
-        <v>346</v>
+      <c r="A31" s="110" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -10304,14 +10694,14 @@
       <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="5.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="116" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="116" width="14.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="116" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="117" width="52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="116" width="9.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="111" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="111" width="14.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="111" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="112" width="52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="111" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="61" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10319,45 +10709,45 @@
         <v>83</v>
       </c>
       <c r="C1" s="61" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>348</v>
-      </c>
-      <c r="E1" s="118"/>
+        <v>383</v>
+      </c>
+      <c r="E1" s="113"/>
     </row>
     <row r="2" s="61" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E2" s="118"/>
+      <c r="E2" s="113"/>
     </row>
     <row r="3" s="61" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="61" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>349</v>
-      </c>
-      <c r="E3" s="118"/>
+        <v>384</v>
+      </c>
+      <c r="E3" s="113"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="116" t="s">
-        <v>350</v>
-      </c>
-      <c r="C4" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E4" s="117" t="s">
-        <v>352</v>
+      <c r="B4" s="111" t="s">
+        <v>385</v>
+      </c>
+      <c r="C4" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E4" s="112" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="54" t="s">
-        <v>353</v>
-      </c>
-      <c r="C5" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E5" s="112" t="s">
-        <v>354</v>
+        <v>388</v>
+      </c>
+      <c r="C5" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E5" s="107" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="8" s="61" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10365,30 +10755,30 @@
         <v>2</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>355</v>
-      </c>
-      <c r="E8" s="118"/>
+        <v>390</v>
+      </c>
+      <c r="E8" s="113"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="54" t="s">
-        <v>356</v>
+        <v>391</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>357</v>
-      </c>
-      <c r="E9" s="112" t="s">
-        <v>358</v>
+        <v>392</v>
+      </c>
+      <c r="E9" s="107" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="54" t="s">
-        <v>359</v>
+        <v>394</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>357</v>
-      </c>
-      <c r="E10" s="112" t="s">
-        <v>360</v>
+        <v>392</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="14" s="61" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10396,22 +10786,22 @@
         <v>3</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>361</v>
-      </c>
-      <c r="E14" s="118"/>
+        <v>396</v>
+      </c>
+      <c r="E14" s="113"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="116" t="s">
-        <v>362</v>
-      </c>
-      <c r="C15" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="D15" s="116" t="s">
-        <v>363</v>
-      </c>
-      <c r="E15" s="117" t="s">
-        <v>364</v>
+      <c r="B15" s="111" t="s">
+        <v>397</v>
+      </c>
+      <c r="C15" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="D15" s="111" t="s">
+        <v>398</v>
+      </c>
+      <c r="E15" s="112" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10419,62 +10809,62 @@
         <v>4</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>365</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="116" t="s">
-        <v>366</v>
-      </c>
-      <c r="C18" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E18" s="117" t="s">
-        <v>367</v>
+      <c r="B18" s="111" t="s">
+        <v>401</v>
+      </c>
+      <c r="C18" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E18" s="112" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="116" t="s">
-        <v>368</v>
-      </c>
-      <c r="C19" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="D19" s="116" t="s">
-        <v>369</v>
+      <c r="B19" s="111" t="s">
+        <v>403</v>
+      </c>
+      <c r="C19" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="D19" s="111" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="116" t="s">
-        <v>370</v>
-      </c>
-      <c r="C20" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E20" s="117" t="s">
-        <v>371</v>
+      <c r="B20" s="111" t="s">
+        <v>405</v>
+      </c>
+      <c r="C20" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E20" s="112" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="116" t="s">
-        <v>372</v>
-      </c>
-      <c r="C21" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="D21" s="116" t="s">
-        <v>373</v>
+      <c r="B21" s="111" t="s">
+        <v>407</v>
+      </c>
+      <c r="C21" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="D21" s="111" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="116" t="s">
-        <v>374</v>
-      </c>
-      <c r="C22" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E22" s="117" t="s">
-        <v>375</v>
+      <c r="B22" s="111" t="s">
+        <v>409</v>
+      </c>
+      <c r="C22" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E22" s="112" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10482,142 +10872,142 @@
         <v>5</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>376</v>
-      </c>
-      <c r="C24" s="116" t="s">
-        <v>377</v>
+        <v>411</v>
+      </c>
+      <c r="C24" s="111" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="116" t="s">
-        <v>378</v>
-      </c>
-      <c r="C25" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E25" s="117" t="s">
-        <v>379</v>
+      <c r="B25" s="111" t="s">
+        <v>413</v>
+      </c>
+      <c r="C25" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E25" s="112" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="116" t="s">
-        <v>380</v>
-      </c>
-      <c r="C26" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E26" s="117" t="s">
-        <v>381</v>
+      <c r="B26" s="111" t="s">
+        <v>415</v>
+      </c>
+      <c r="C26" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E26" s="112" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="116" t="s">
-        <v>382</v>
-      </c>
-      <c r="C27" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E27" s="117" t="s">
-        <v>383</v>
+      <c r="B27" s="111" t="s">
+        <v>417</v>
+      </c>
+      <c r="C27" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E27" s="112" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="116" t="s">
-        <v>384</v>
-      </c>
-      <c r="C28" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E28" s="117" t="s">
-        <v>385</v>
+      <c r="B28" s="111" t="s">
+        <v>419</v>
+      </c>
+      <c r="C28" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E28" s="112" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="116" t="s">
+      <c r="B29" s="111" t="s">
+        <v>421</v>
+      </c>
+      <c r="C29" s="111" t="s">
         <v>386</v>
       </c>
-      <c r="C29" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E29" s="117" t="s">
-        <v>387</v>
+      <c r="E29" s="112" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="116" t="s">
-        <v>388</v>
-      </c>
-      <c r="C30" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E30" s="117" t="s">
-        <v>389</v>
+      <c r="B30" s="111" t="s">
+        <v>423</v>
+      </c>
+      <c r="C30" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E30" s="112" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="116" t="s">
-        <v>390</v>
-      </c>
-      <c r="C31" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E31" s="117" t="s">
-        <v>391</v>
+      <c r="B31" s="111" t="s">
+        <v>425</v>
+      </c>
+      <c r="C31" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E31" s="112" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="116" t="s">
-        <v>392</v>
-      </c>
-      <c r="C32" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E32" s="117" t="s">
-        <v>393</v>
+      <c r="B32" s="111" t="s">
+        <v>427</v>
+      </c>
+      <c r="C32" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E32" s="112" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="116" t="s">
-        <v>394</v>
-      </c>
-      <c r="C33" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E33" s="117" t="s">
-        <v>395</v>
+      <c r="B33" s="111" t="s">
+        <v>429</v>
+      </c>
+      <c r="C33" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E33" s="112" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="116" t="s">
-        <v>396</v>
-      </c>
-      <c r="C34" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E34" s="117" t="s">
-        <v>397</v>
+      <c r="B34" s="111" t="s">
+        <v>431</v>
+      </c>
+      <c r="C34" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E34" s="112" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="116" t="s">
-        <v>372</v>
-      </c>
-      <c r="C35" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E35" s="117" t="s">
-        <v>398</v>
+      <c r="B35" s="111" t="s">
+        <v>407</v>
+      </c>
+      <c r="C35" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E35" s="112" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="116" t="s">
-        <v>399</v>
-      </c>
-      <c r="C36" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E36" s="117" t="s">
-        <v>400</v>
+      <c r="B36" s="111" t="s">
+        <v>434</v>
+      </c>
+      <c r="C36" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E36" s="112" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10625,10 +11015,10 @@
         <v>6</v>
       </c>
       <c r="B38" s="61" t="s">
-        <v>401</v>
-      </c>
-      <c r="C38" s="116" t="s">
-        <v>402</v>
+        <v>436</v>
+      </c>
+      <c r="C38" s="111" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10636,51 +11026,51 @@
         <v>7</v>
       </c>
       <c r="B41" s="61" t="s">
-        <v>403</v>
+        <v>438</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="116" t="s">
-        <v>404</v>
-      </c>
-      <c r="C42" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E42" s="117" t="s">
-        <v>405</v>
+      <c r="B42" s="111" t="s">
+        <v>439</v>
+      </c>
+      <c r="C42" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E42" s="112" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="116" t="n">
+      <c r="B43" s="111" t="n">
         <v>8</v>
       </c>
-      <c r="C43" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E43" s="117" t="s">
-        <v>406</v>
+      <c r="C43" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E43" s="112" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="116" t="n">
+      <c r="B44" s="111" t="n">
         <v>73</v>
       </c>
-      <c r="C44" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E44" s="117" t="s">
-        <v>407</v>
+      <c r="C44" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E44" s="112" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="116" t="n">
+      <c r="B45" s="111" t="n">
         <v>74</v>
       </c>
-      <c r="C45" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E45" s="117" t="s">
-        <v>408</v>
+      <c r="C45" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E45" s="112" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10688,99 +11078,99 @@
         <v>13</v>
       </c>
       <c r="B49" s="61" t="s">
-        <v>409</v>
+        <v>444</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="119" t="s">
-        <v>410</v>
-      </c>
-      <c r="C50" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E50" s="117" t="s">
-        <v>411</v>
+      <c r="B50" s="114" t="s">
+        <v>445</v>
+      </c>
+      <c r="C50" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E50" s="112" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="119" t="s">
-        <v>412</v>
-      </c>
-      <c r="C51" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E51" s="117" t="s">
-        <v>413</v>
+      <c r="B51" s="114" t="s">
+        <v>447</v>
+      </c>
+      <c r="C51" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E51" s="112" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="119" t="s">
-        <v>414</v>
-      </c>
-      <c r="C52" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E52" s="117" t="s">
-        <v>415</v>
+      <c r="B52" s="114" t="s">
+        <v>449</v>
+      </c>
+      <c r="C52" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E52" s="112" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="119" t="s">
-        <v>416</v>
-      </c>
-      <c r="C53" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E53" s="117" t="s">
-        <v>417</v>
+      <c r="B53" s="114" t="s">
+        <v>451</v>
+      </c>
+      <c r="C53" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E53" s="112" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="119" t="s">
-        <v>418</v>
-      </c>
-      <c r="C54" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E54" s="117" t="s">
-        <v>419</v>
+      <c r="B54" s="114" t="s">
+        <v>453</v>
+      </c>
+      <c r="C54" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E54" s="112" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="119" t="s">
-        <v>420</v>
-      </c>
-      <c r="C55" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E55" s="117" t="s">
-        <v>421</v>
+      <c r="B55" s="114" t="s">
+        <v>455</v>
+      </c>
+      <c r="C55" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E55" s="112" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="119" t="s">
-        <v>422</v>
-      </c>
-      <c r="C56" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E56" s="117" t="s">
-        <v>423</v>
+      <c r="B56" s="114" t="s">
+        <v>457</v>
+      </c>
+      <c r="C56" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E56" s="112" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="119" t="n">
+      <c r="B57" s="114" t="n">
         <v>175</v>
       </c>
-      <c r="C57" s="116" t="s">
-        <v>351</v>
-      </c>
-      <c r="E57" s="117" t="s">
-        <v>424</v>
+      <c r="C57" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E57" s="112" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="120"/>
+      <c r="B58" s="115"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>